<commit_message>
Write scripts to add data into a sqlite database
</commit_message>
<xml_diff>
--- a/processed_data/_2013-2014.xlsx
+++ b/processed_data/_2013-2014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Fall 2013" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6200" uniqueCount="2097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8464" uniqueCount="2097">
   <si>
     <t>AcadYr</t>
   </si>
@@ -6667,8 +6667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P282"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9229,6 +9229,9 @@
         <v>22</v>
       </c>
       <c r="N51" s="1">
+        <v>0</v>
+      </c>
+      <c r="O51" s="1">
         <v>0</v>
       </c>
       <c r="P51" s="1" t="s">
@@ -33427,8 +33430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>